<commit_message>
Reorganizacao espec interface remuneracao
</commit_message>
<xml_diff>
--- a/espec002_remuneracao-servidores/static/leiaute_tabelas_navegacao_filtros.xlsx
+++ b/espec002_remuneracao-servidores/static/leiaute_tabelas_navegacao_filtros.xlsx
@@ -242,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -276,6 +276,9 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -365,6 +368,234 @@
         <a:xfrm>
           <a:off x="581024" y="3962400"/>
           <a:ext cx="12011025" cy="438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2781256</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>352385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3038475" y="1171575"/>
+          <a:ext cx="352381" cy="323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>793937</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1104856</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>333335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4241987" y="1190625"/>
+          <a:ext cx="310919" cy="285710"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2114506</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>333335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6315075" y="1152525"/>
+          <a:ext cx="352381" cy="323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2447881</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>371435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8829675" y="1190625"/>
+          <a:ext cx="352381" cy="323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1428751</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1677521</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10658476" y="1209675"/>
+          <a:ext cx="248770" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1725145</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12439650" y="1228725"/>
+          <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -642,7 +873,7 @@
   <dimension ref="B6:G14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +906,10 @@
       <c r="E7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Altera especificação para envio à Prodemge
</commit_message>
<xml_diff>
--- a/espec002_remuneracao-servidores/static/leiaute_tabelas_navegacao_filtros.xlsx
+++ b/espec002_remuneracao-servidores/static/leiaute_tabelas_navegacao_filtros.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m752587\projects\especificacoes-portal-transparencia\espec002_remuneracao-servidores\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m13368964\Documents\Documents\CGE\Projetos-Transparencia-Ativa\especificacoes-portal-transparencia\espec002_remuneracao-servidores\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Servidor</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Masp</t>
   </si>
   <si>
-    <t>Cargo</t>
-  </si>
-  <si>
     <t>Remuneração Bruta</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>PAULO PEDRO DE ALMEIDA</t>
-  </si>
-  <si>
-    <t>ANALISTA DE GESTAO ARTISTICA</t>
   </si>
   <si>
     <t>TOTAL GERAL:</t>
@@ -271,14 +265,14 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -308,8 +302,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>142752</xdr:rowOff>
     </xdr:to>
@@ -329,7 +323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="561974" y="114300"/>
-          <a:ext cx="12182475" cy="980952"/>
+          <a:ext cx="9982201" cy="980952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -341,13 +335,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1628774</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>133295</xdr:rowOff>
     </xdr:to>
@@ -366,8 +360,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581024" y="3962400"/>
-          <a:ext cx="12011025" cy="438095"/>
+          <a:off x="581025" y="3810000"/>
+          <a:ext cx="9934576" cy="438095"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -379,15 +373,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:colOff>1724025</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2781256</xdr:colOff>
+      <xdr:colOff>2076406</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>352385</xdr:rowOff>
+      <xdr:rowOff>361910</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -404,7 +398,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3038475" y="1171575"/>
+          <a:off x="2333625" y="1181100"/>
           <a:ext cx="352381" cy="323810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -417,15 +411,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>793937</xdr:colOff>
+      <xdr:colOff>803463</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1104856</xdr:colOff>
+      <xdr:colOff>1047751</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>333335</xdr:rowOff>
+      <xdr:rowOff>310206</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -442,8 +436,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4241987" y="1190625"/>
-          <a:ext cx="310919" cy="285710"/>
+          <a:off x="4251513" y="1228725"/>
+          <a:ext cx="244288" cy="224481"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -457,49 +451,11 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2114506</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>333335</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagem 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6315075" y="1152525"/>
-          <a:ext cx="352381" cy="323810"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2095500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2447881</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>371435</xdr:rowOff>
     </xdr:to>
@@ -518,7 +474,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8829675" y="1190625"/>
+          <a:off x="6315075" y="1190625"/>
           <a:ext cx="352381" cy="323810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -530,16 +486,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1428751</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1352551</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1677521</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1601321</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -556,7 +512,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10658476" y="1209675"/>
+          <a:off x="8401051" y="1219200"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -568,13 +524,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1476375</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1725145</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
@@ -870,30 +826,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:G14"/>
+  <dimension ref="B6:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
@@ -901,145 +855,125 @@
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="12" t="s">
+    </row>
+    <row r="8" spans="2:6" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C8" s="3">
         <v>10358737</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5939.01</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6115.14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="F8" s="4">
-        <v>5939.01</v>
-      </c>
-      <c r="G8" s="4">
-        <v>6115.14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>13577564</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1357.49</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2374.13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1357.49</v>
-      </c>
-      <c r="G9" s="4">
-        <v>2374.13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>10357358</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
         <v>2372.66</v>
       </c>
-      <c r="G10" s="4">
+      <c r="F10" s="4">
         <v>1866.08</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>10358026</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
         <v>5322.32</v>
       </c>
-      <c r="G11" s="4">
+      <c r="F11" s="4">
         <v>4183.66</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
         <v>9789884</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4">
+        <v>6650.36</v>
       </c>
       <c r="F12" s="4">
-        <v>6650.36</v>
-      </c>
-      <c r="G12" s="4">
         <v>6750.87</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+    <row r="13" spans="2:6" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="6">
+        <f>SUM(E8:E12)</f>
+        <v>21641.84</v>
+      </c>
       <c r="F13" s="6">
         <f>SUM(F8:F12)</f>
-        <v>21641.84</v>
-      </c>
-      <c r="G13" s="6">
-        <f>SUM(G8:G12)</f>
         <v>21289.88</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>